<commit_message>
Change container length width values and pass container info to visualizer.
</commit_message>
<xml_diff>
--- a/LoadBuilder/Data/container_dimensions.xlsx
+++ b/LoadBuilder/Data/container_dimensions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alperkilinc/Desktop/KU/INDR491/LoadBuilder/LoadBuilder/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA93CC-30E5-234A-B9A6-00313B3C3F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3CEC77-00A6-1E40-9600-E0B395689B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="3260" windowWidth="27640" windowHeight="16940" xr2:uid="{6104068A-A477-E849-A5F0-4C67F52013BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,10 +448,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
+        <v>235</v>
+      </c>
+      <c r="C2" s="1">
         <v>590</v>
-      </c>
-      <c r="C2" s="1">
-        <v>235</v>
       </c>
       <c r="D2" s="1">
         <v>239</v>
@@ -462,10 +462,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
+        <v>235</v>
+      </c>
+      <c r="C3" s="1">
         <v>1204</v>
-      </c>
-      <c r="C3" s="1">
-        <v>235</v>
       </c>
       <c r="D3" s="1">
         <v>239</v>
@@ -476,10 +476,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
+        <v>235</v>
+      </c>
+      <c r="C4" s="1">
         <v>1204</v>
-      </c>
-      <c r="C4" s="1">
-        <v>235</v>
       </c>
       <c r="D4" s="1">
         <v>269</v>
@@ -490,10 +490,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
+        <v>244</v>
+      </c>
+      <c r="C5" s="1">
         <v>1359</v>
-      </c>
-      <c r="C5" s="1">
-        <v>244</v>
       </c>
       <c r="D5" s="1">
         <v>269</v>
@@ -504,10 +504,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
+        <v>248</v>
+      </c>
+      <c r="C6" s="1">
         <v>1360</v>
-      </c>
-      <c r="C6" s="1">
-        <v>248</v>
       </c>
       <c r="D6" s="1">
         <v>270</v>

</xml_diff>